<commit_message>
Efficiency update and progress bar. Slight changes to data saving
</commit_message>
<xml_diff>
--- a/excel_export.xlsx
+++ b/excel_export.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="20">
   <si>
     <t>0,0</t>
   </si>
@@ -431,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K760"/>
+  <dimension ref="A1:K804"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -889,7 +889,7 @@
         <v>16</v>
       </c>
       <c r="K13">
-        <v>37262</v>
+        <v>37911</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -924,7 +924,7 @@
         <v>11</v>
       </c>
       <c r="K14">
-        <v>4217</v>
+        <v>4278</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -959,7 +959,7 @@
         <v>13</v>
       </c>
       <c r="K15">
-        <v>1089</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -994,7 +994,7 @@
         <v>17</v>
       </c>
       <c r="K16">
-        <v>1002</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1029,7 +1029,7 @@
         <v>11</v>
       </c>
       <c r="K17">
-        <v>4549</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1064,7 +1064,7 @@
         <v>17</v>
       </c>
       <c r="K18">
-        <v>1298</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1099,7 +1099,7 @@
         <v>15</v>
       </c>
       <c r="K19">
-        <v>2870</v>
+        <v>2939</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1134,7 +1134,7 @@
         <v>11</v>
       </c>
       <c r="K20">
-        <v>498</v>
+        <v>509</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1169,7 +1169,7 @@
         <v>13</v>
       </c>
       <c r="K21">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1204,7 +1204,7 @@
         <v>11</v>
       </c>
       <c r="K22">
-        <v>4250</v>
+        <v>4329</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1239,7 +1239,7 @@
         <v>14</v>
       </c>
       <c r="K23">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1379,7 +1379,7 @@
         <v>13</v>
       </c>
       <c r="K27">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1449,7 +1449,7 @@
         <v>18</v>
       </c>
       <c r="K29">
-        <v>4456</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1484,7 +1484,7 @@
         <v>15</v>
       </c>
       <c r="K30">
-        <v>626</v>
+        <v>636</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1519,7 +1519,7 @@
         <v>13</v>
       </c>
       <c r="K31">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1554,7 +1554,7 @@
         <v>13</v>
       </c>
       <c r="K32">
-        <v>8293</v>
+        <v>8360</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1589,7 +1589,7 @@
         <v>19</v>
       </c>
       <c r="K33">
-        <v>1357</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1624,7 +1624,7 @@
         <v>14</v>
       </c>
       <c r="K34">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1694,7 +1694,7 @@
         <v>13</v>
       </c>
       <c r="K36">
-        <v>540</v>
+        <v>551</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -1729,7 +1729,7 @@
         <v>11</v>
       </c>
       <c r="K37">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1764,7 +1764,7 @@
         <v>17</v>
       </c>
       <c r="K38">
-        <v>646</v>
+        <v>657</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1799,7 +1799,7 @@
         <v>19</v>
       </c>
       <c r="K39">
-        <v>1174</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -1834,7 +1834,7 @@
         <v>18</v>
       </c>
       <c r="K40">
-        <v>395</v>
+        <v>403</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -1869,7 +1869,7 @@
         <v>15</v>
       </c>
       <c r="K41">
-        <v>4307</v>
+        <v>4459</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -1904,7 +1904,7 @@
         <v>12</v>
       </c>
       <c r="K42">
-        <v>717</v>
+        <v>745</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -1939,7 +1939,7 @@
         <v>17</v>
       </c>
       <c r="K43">
-        <v>633</v>
+        <v>638</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -1974,7 +1974,7 @@
         <v>12</v>
       </c>
       <c r="K44">
-        <v>799</v>
+        <v>817</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2009,7 +2009,7 @@
         <v>17</v>
       </c>
       <c r="K45">
-        <v>710</v>
+        <v>715</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2114,7 +2114,7 @@
         <v>17</v>
       </c>
       <c r="K48">
-        <v>653</v>
+        <v>664</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2184,7 +2184,7 @@
         <v>19</v>
       </c>
       <c r="K50">
-        <v>1597</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2219,7 +2219,7 @@
         <v>17</v>
       </c>
       <c r="K51">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2254,7 +2254,7 @@
         <v>13</v>
       </c>
       <c r="K52">
-        <v>658</v>
+        <v>668</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2289,7 +2289,7 @@
         <v>17</v>
       </c>
       <c r="K53">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2429,7 +2429,7 @@
         <v>12</v>
       </c>
       <c r="K57">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -2464,7 +2464,7 @@
         <v>17</v>
       </c>
       <c r="K58">
-        <v>1144</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -2499,7 +2499,7 @@
         <v>13</v>
       </c>
       <c r="K59">
-        <v>1272</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -2534,7 +2534,7 @@
         <v>19</v>
       </c>
       <c r="K60">
-        <v>1338</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -2569,7 +2569,7 @@
         <v>12</v>
       </c>
       <c r="K61">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -2604,7 +2604,7 @@
         <v>14</v>
       </c>
       <c r="K62">
-        <v>513</v>
+        <v>527</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -2639,7 +2639,7 @@
         <v>19</v>
       </c>
       <c r="K63">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -2709,7 +2709,7 @@
         <v>12</v>
       </c>
       <c r="K65">
-        <v>353</v>
+        <v>366</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -2744,7 +2744,7 @@
         <v>14</v>
       </c>
       <c r="K66">
-        <v>1166</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -2779,7 +2779,7 @@
         <v>19</v>
       </c>
       <c r="K67">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -2814,7 +2814,7 @@
         <v>18</v>
       </c>
       <c r="K68">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -2849,7 +2849,7 @@
         <v>18</v>
       </c>
       <c r="K69">
-        <v>789</v>
+        <v>812</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -2884,7 +2884,7 @@
         <v>19</v>
       </c>
       <c r="K70">
-        <v>523</v>
+        <v>540</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -2919,7 +2919,7 @@
         <v>12</v>
       </c>
       <c r="K71">
-        <v>383</v>
+        <v>388</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -2954,7 +2954,7 @@
         <v>18</v>
       </c>
       <c r="K72">
-        <v>586</v>
+        <v>589</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -2989,7 +2989,7 @@
         <v>18</v>
       </c>
       <c r="K73">
-        <v>1480</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -3199,7 +3199,7 @@
         <v>18</v>
       </c>
       <c r="K79">
-        <v>1317</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -3234,7 +3234,7 @@
         <v>14</v>
       </c>
       <c r="K80">
-        <v>319</v>
+        <v>329</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -3269,7 +3269,7 @@
         <v>19</v>
       </c>
       <c r="K81">
-        <v>313</v>
+        <v>321</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -3304,7 +3304,7 @@
         <v>13</v>
       </c>
       <c r="K82">
-        <v>264</v>
+        <v>272</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -3339,7 +3339,7 @@
         <v>15</v>
       </c>
       <c r="K83">
-        <v>642</v>
+        <v>659</v>
       </c>
     </row>
     <row r="84" spans="1:11">
@@ -3374,7 +3374,7 @@
         <v>17</v>
       </c>
       <c r="K84">
-        <v>4273</v>
+        <v>4352</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -3444,7 +3444,7 @@
         <v>11</v>
       </c>
       <c r="K86">
-        <v>1354</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -3479,7 +3479,7 @@
         <v>12</v>
       </c>
       <c r="K87">
-        <v>344</v>
+        <v>349</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -3619,7 +3619,7 @@
         <v>11</v>
       </c>
       <c r="K91">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -3654,7 +3654,7 @@
         <v>18</v>
       </c>
       <c r="K92">
-        <v>399</v>
+        <v>413</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -3689,7 +3689,7 @@
         <v>14</v>
       </c>
       <c r="K93">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -3759,7 +3759,7 @@
         <v>19</v>
       </c>
       <c r="K95">
-        <v>313</v>
+        <v>318</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -3794,7 +3794,7 @@
         <v>13</v>
       </c>
       <c r="K96">
-        <v>689</v>
+        <v>702</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -3829,7 +3829,7 @@
         <v>15</v>
       </c>
       <c r="K97">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -3864,7 +3864,7 @@
         <v>17</v>
       </c>
       <c r="K98">
-        <v>652</v>
+        <v>667</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -3899,7 +3899,7 @@
         <v>14</v>
       </c>
       <c r="K99">
-        <v>755</v>
+        <v>768</v>
       </c>
     </row>
     <row r="100" spans="1:11">
@@ -3934,7 +3934,7 @@
         <v>17</v>
       </c>
       <c r="K100">
-        <v>548</v>
+        <v>556</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -4004,7 +4004,7 @@
         <v>19</v>
       </c>
       <c r="K102">
-        <v>1289</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="103" spans="1:11">
@@ -4039,7 +4039,7 @@
         <v>13</v>
       </c>
       <c r="K103">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="104" spans="1:11">
@@ -4074,7 +4074,7 @@
         <v>19</v>
       </c>
       <c r="K104">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="105" spans="1:11">
@@ -4109,7 +4109,7 @@
         <v>19</v>
       </c>
       <c r="K105">
-        <v>654</v>
+        <v>668</v>
       </c>
     </row>
     <row r="106" spans="1:11">
@@ -4144,7 +4144,7 @@
         <v>14</v>
       </c>
       <c r="K106">
-        <v>588</v>
+        <v>594</v>
       </c>
     </row>
     <row r="107" spans="1:11">
@@ -4179,7 +4179,7 @@
         <v>11</v>
       </c>
       <c r="K107">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="108" spans="1:11">
@@ -4214,7 +4214,7 @@
         <v>18</v>
       </c>
       <c r="K108">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="109" spans="1:11">
@@ -4249,7 +4249,7 @@
         <v>14</v>
       </c>
       <c r="K109">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="110" spans="1:11">
@@ -4284,7 +4284,7 @@
         <v>14</v>
       </c>
       <c r="K110">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="111" spans="1:11">
@@ -4319,7 +4319,7 @@
         <v>13</v>
       </c>
       <c r="K111">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="1:11">
@@ -4354,7 +4354,7 @@
         <v>15</v>
       </c>
       <c r="K112">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="113" spans="1:11">
@@ -4389,7 +4389,7 @@
         <v>12</v>
       </c>
       <c r="K113">
-        <v>802</v>
+        <v>831</v>
       </c>
     </row>
     <row r="114" spans="1:11">
@@ -4424,7 +4424,7 @@
         <v>13</v>
       </c>
       <c r="K114">
-        <v>1315</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="115" spans="1:11">
@@ -4494,7 +4494,7 @@
         <v>19</v>
       </c>
       <c r="K116">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
     <row r="117" spans="1:11">
@@ -4529,7 +4529,7 @@
         <v>15</v>
       </c>
       <c r="K117">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="118" spans="1:11">
@@ -4564,7 +4564,7 @@
         <v>18</v>
       </c>
       <c r="K118">
-        <v>885</v>
+        <v>895</v>
       </c>
     </row>
     <row r="119" spans="1:11">
@@ -4599,7 +4599,7 @@
         <v>18</v>
       </c>
       <c r="K119">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="120" spans="1:11">
@@ -4669,7 +4669,7 @@
         <v>17</v>
       </c>
       <c r="K121">
-        <v>261</v>
+        <v>271</v>
       </c>
     </row>
     <row r="122" spans="1:11">
@@ -4704,7 +4704,7 @@
         <v>11</v>
       </c>
       <c r="K122">
-        <v>663</v>
+        <v>676</v>
       </c>
     </row>
     <row r="123" spans="1:11">
@@ -4739,7 +4739,7 @@
         <v>15</v>
       </c>
       <c r="K123">
-        <v>392</v>
+        <v>403</v>
       </c>
     </row>
     <row r="124" spans="1:11">
@@ -4774,7 +4774,7 @@
         <v>15</v>
       </c>
       <c r="K124">
-        <v>693</v>
+        <v>706</v>
       </c>
     </row>
     <row r="125" spans="1:11">
@@ -4879,7 +4879,7 @@
         <v>15</v>
       </c>
       <c r="K127">
-        <v>559</v>
+        <v>572</v>
       </c>
     </row>
     <row r="128" spans="1:11">
@@ -4914,7 +4914,7 @@
         <v>11</v>
       </c>
       <c r="K128">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="129" spans="1:11">
@@ -4949,7 +4949,7 @@
         <v>18</v>
       </c>
       <c r="K129">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="130" spans="1:11">
@@ -4984,7 +4984,7 @@
         <v>13</v>
       </c>
       <c r="K130">
-        <v>785</v>
+        <v>793</v>
       </c>
     </row>
     <row r="131" spans="1:11">
@@ -5019,7 +5019,7 @@
         <v>17</v>
       </c>
       <c r="K131">
-        <v>393</v>
+        <v>398</v>
       </c>
     </row>
     <row r="132" spans="1:11">
@@ -5054,7 +5054,7 @@
         <v>19</v>
       </c>
       <c r="K132">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="133" spans="1:11">
@@ -5089,7 +5089,7 @@
         <v>11</v>
       </c>
       <c r="K133">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="134" spans="1:11">
@@ -5124,7 +5124,7 @@
         <v>13</v>
       </c>
       <c r="K134">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="135" spans="1:11">
@@ -5194,7 +5194,7 @@
         <v>13</v>
       </c>
       <c r="K136">
-        <v>377</v>
+        <v>383</v>
       </c>
     </row>
     <row r="137" spans="1:11">
@@ -5229,7 +5229,7 @@
         <v>12</v>
       </c>
       <c r="K137">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="138" spans="1:11">
@@ -5264,7 +5264,7 @@
         <v>15</v>
       </c>
       <c r="K138">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="139" spans="1:11">
@@ -5334,7 +5334,7 @@
         <v>12</v>
       </c>
       <c r="K140">
-        <v>386</v>
+        <v>392</v>
       </c>
     </row>
     <row r="141" spans="1:11">
@@ -5369,7 +5369,7 @@
         <v>11</v>
       </c>
       <c r="K141">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="142" spans="1:11">
@@ -5404,7 +5404,7 @@
         <v>13</v>
       </c>
       <c r="K142">
-        <v>496</v>
+        <v>504</v>
       </c>
     </row>
     <row r="143" spans="1:11">
@@ -5439,7 +5439,7 @@
         <v>18</v>
       </c>
       <c r="K143">
-        <v>383</v>
+        <v>395</v>
       </c>
     </row>
     <row r="144" spans="1:11">
@@ -5509,7 +5509,7 @@
         <v>17</v>
       </c>
       <c r="K145">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="146" spans="1:11">
@@ -5614,7 +5614,7 @@
         <v>17</v>
       </c>
       <c r="K148">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="149" spans="1:11">
@@ -5649,7 +5649,7 @@
         <v>14</v>
       </c>
       <c r="K149">
-        <v>595</v>
+        <v>626</v>
       </c>
     </row>
     <row r="150" spans="1:11">
@@ -5684,7 +5684,7 @@
         <v>12</v>
       </c>
       <c r="K150">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="151" spans="1:11">
@@ -5859,7 +5859,7 @@
         <v>13</v>
       </c>
       <c r="K155">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="156" spans="1:11">
@@ -5894,7 +5894,7 @@
         <v>12</v>
       </c>
       <c r="K156">
-        <v>1405</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="157" spans="1:11">
@@ -5929,7 +5929,7 @@
         <v>15</v>
       </c>
       <c r="K157">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="158" spans="1:11">
@@ -5964,7 +5964,7 @@
         <v>17</v>
       </c>
       <c r="K158">
-        <v>535</v>
+        <v>539</v>
       </c>
     </row>
     <row r="159" spans="1:11">
@@ -5999,7 +5999,7 @@
         <v>12</v>
       </c>
       <c r="K159">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="160" spans="1:11">
@@ -6034,7 +6034,7 @@
         <v>18</v>
       </c>
       <c r="K160">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="161" spans="1:11">
@@ -6069,7 +6069,7 @@
         <v>15</v>
       </c>
       <c r="K161">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="162" spans="1:11">
@@ -6104,7 +6104,7 @@
         <v>18</v>
       </c>
       <c r="K162">
-        <v>644</v>
+        <v>655</v>
       </c>
     </row>
     <row r="163" spans="1:11">
@@ -6139,7 +6139,7 @@
         <v>14</v>
       </c>
       <c r="K163">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="164" spans="1:11">
@@ -6209,7 +6209,7 @@
         <v>11</v>
       </c>
       <c r="K165">
-        <v>771</v>
+        <v>778</v>
       </c>
     </row>
     <row r="166" spans="1:11">
@@ -6244,7 +6244,7 @@
         <v>15</v>
       </c>
       <c r="K166">
-        <v>266</v>
+        <v>274</v>
       </c>
     </row>
     <row r="167" spans="1:11">
@@ -6314,7 +6314,7 @@
         <v>13</v>
       </c>
       <c r="K168">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="169" spans="1:11">
@@ -6349,7 +6349,7 @@
         <v>17</v>
       </c>
       <c r="K169">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="170" spans="1:11">
@@ -6419,7 +6419,7 @@
         <v>13</v>
       </c>
       <c r="K171">
-        <v>629</v>
+        <v>639</v>
       </c>
     </row>
     <row r="172" spans="1:11">
@@ -6489,7 +6489,7 @@
         <v>15</v>
       </c>
       <c r="K173">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="174" spans="1:11">
@@ -6524,7 +6524,7 @@
         <v>17</v>
       </c>
       <c r="K174">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="175" spans="1:11">
@@ -6559,7 +6559,7 @@
         <v>12</v>
       </c>
       <c r="K175">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="176" spans="1:11">
@@ -6594,7 +6594,7 @@
         <v>14</v>
       </c>
       <c r="K176">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="177" spans="1:11">
@@ -6629,7 +6629,7 @@
         <v>12</v>
       </c>
       <c r="K177">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="178" spans="1:11">
@@ -6664,7 +6664,7 @@
         <v>19</v>
       </c>
       <c r="K178">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="179" spans="1:11">
@@ -6734,7 +6734,7 @@
         <v>17</v>
       </c>
       <c r="K180">
-        <v>1276</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="181" spans="1:11">
@@ -6769,7 +6769,7 @@
         <v>11</v>
       </c>
       <c r="K181">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="182" spans="1:11">
@@ -6804,7 +6804,7 @@
         <v>12</v>
       </c>
       <c r="K182">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="183" spans="1:11">
@@ -6839,7 +6839,7 @@
         <v>18</v>
       </c>
       <c r="K183">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="184" spans="1:11">
@@ -6874,7 +6874,7 @@
         <v>13</v>
       </c>
       <c r="K184">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="185" spans="1:11">
@@ -6944,7 +6944,7 @@
         <v>14</v>
       </c>
       <c r="K186">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="187" spans="1:11">
@@ -6979,7 +6979,7 @@
         <v>11</v>
       </c>
       <c r="K187">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="188" spans="1:11">
@@ -7014,7 +7014,7 @@
         <v>18</v>
       </c>
       <c r="K188">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="189" spans="1:11">
@@ -7049,7 +7049,7 @@
         <v>18</v>
       </c>
       <c r="K189">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="190" spans="1:11">
@@ -7084,7 +7084,7 @@
         <v>13</v>
       </c>
       <c r="K190">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="191" spans="1:11">
@@ -7119,7 +7119,7 @@
         <v>18</v>
       </c>
       <c r="K191">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="192" spans="1:11">
@@ -7154,7 +7154,7 @@
         <v>18</v>
       </c>
       <c r="K192">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="193" spans="1:11">
@@ -7259,7 +7259,7 @@
         <v>12</v>
       </c>
       <c r="K195">
-        <v>191</v>
+        <v>205</v>
       </c>
     </row>
     <row r="196" spans="1:11">
@@ -7294,7 +7294,7 @@
         <v>11</v>
       </c>
       <c r="K196">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="197" spans="1:11">
@@ -7329,7 +7329,7 @@
         <v>17</v>
       </c>
       <c r="K197">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="198" spans="1:11">
@@ -7364,7 +7364,7 @@
         <v>18</v>
       </c>
       <c r="K198">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="199" spans="1:11">
@@ -7434,7 +7434,7 @@
         <v>18</v>
       </c>
       <c r="K200">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="201" spans="1:11">
@@ -7469,7 +7469,7 @@
         <v>19</v>
       </c>
       <c r="K201">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="202" spans="1:11">
@@ -7504,7 +7504,7 @@
         <v>11</v>
       </c>
       <c r="K202">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="203" spans="1:11">
@@ -7539,7 +7539,7 @@
         <v>14</v>
       </c>
       <c r="K203">
-        <v>316</v>
+        <v>334</v>
       </c>
     </row>
     <row r="204" spans="1:11">
@@ -7574,7 +7574,7 @@
         <v>19</v>
       </c>
       <c r="K204">
-        <v>314</v>
+        <v>324</v>
       </c>
     </row>
     <row r="205" spans="1:11">
@@ -7609,7 +7609,7 @@
         <v>14</v>
       </c>
       <c r="K205">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="206" spans="1:11">
@@ -7679,7 +7679,7 @@
         <v>19</v>
       </c>
       <c r="K207">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="208" spans="1:11">
@@ -7714,7 +7714,7 @@
         <v>14</v>
       </c>
       <c r="K208">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="209" spans="1:11">
@@ -7749,7 +7749,7 @@
         <v>15</v>
       </c>
       <c r="K209">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="210" spans="1:11">
@@ -7784,7 +7784,7 @@
         <v>15</v>
       </c>
       <c r="K210">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="211" spans="1:11">
@@ -7819,7 +7819,7 @@
         <v>18</v>
       </c>
       <c r="K211">
-        <v>324</v>
+        <v>336</v>
       </c>
     </row>
     <row r="212" spans="1:11">
@@ -7854,7 +7854,7 @@
         <v>15</v>
       </c>
       <c r="K212">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="213" spans="1:11">
@@ -7889,7 +7889,7 @@
         <v>19</v>
       </c>
       <c r="K213">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="214" spans="1:11">
@@ -7924,7 +7924,7 @@
         <v>19</v>
       </c>
       <c r="K214">
-        <v>484</v>
+        <v>493</v>
       </c>
     </row>
     <row r="215" spans="1:11">
@@ -7959,7 +7959,7 @@
         <v>15</v>
       </c>
       <c r="K215">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="216" spans="1:11">
@@ -7994,7 +7994,7 @@
         <v>15</v>
       </c>
       <c r="K216">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="217" spans="1:11">
@@ -8029,7 +8029,7 @@
         <v>15</v>
       </c>
       <c r="K217">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="218" spans="1:11">
@@ -8484,7 +8484,7 @@
         <v>15</v>
       </c>
       <c r="K230">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="231" spans="1:11">
@@ -9499,7 +9499,7 @@
         <v>18</v>
       </c>
       <c r="K259">
-        <v>-17</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="260" spans="1:11">
@@ -14679,7 +14679,7 @@
         <v>13</v>
       </c>
       <c r="K407">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="408" spans="1:11">
@@ -24654,7 +24654,7 @@
         <v>19</v>
       </c>
       <c r="K692">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="693" spans="1:11">
@@ -27034,6 +27034,1546 @@
         <v>14</v>
       </c>
       <c r="K760">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="761" spans="1:11">
+      <c r="A761">
+        <v>0</v>
+      </c>
+      <c r="B761">
+        <v>0</v>
+      </c>
+      <c r="C761">
+        <v>0</v>
+      </c>
+      <c r="D761">
+        <v>0</v>
+      </c>
+      <c r="E761">
+        <v>0</v>
+      </c>
+      <c r="F761">
+        <v>0</v>
+      </c>
+      <c r="G761">
+        <v>-1</v>
+      </c>
+      <c r="H761">
+        <v>0</v>
+      </c>
+      <c r="I761">
+        <v>0</v>
+      </c>
+      <c r="J761" t="s">
+        <v>16</v>
+      </c>
+      <c r="K761">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="762" spans="1:11">
+      <c r="A762">
+        <v>0</v>
+      </c>
+      <c r="B762">
+        <v>0</v>
+      </c>
+      <c r="C762">
+        <v>0</v>
+      </c>
+      <c r="D762">
+        <v>0</v>
+      </c>
+      <c r="E762">
+        <v>1</v>
+      </c>
+      <c r="F762">
+        <v>0</v>
+      </c>
+      <c r="G762">
+        <v>-1</v>
+      </c>
+      <c r="H762">
+        <v>0</v>
+      </c>
+      <c r="I762">
+        <v>-1</v>
+      </c>
+      <c r="J762" t="s">
+        <v>11</v>
+      </c>
+      <c r="K762">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="763" spans="1:11">
+      <c r="A763">
+        <v>0</v>
+      </c>
+      <c r="B763">
+        <v>-1</v>
+      </c>
+      <c r="C763">
+        <v>0</v>
+      </c>
+      <c r="D763">
+        <v>0</v>
+      </c>
+      <c r="E763">
+        <v>1</v>
+      </c>
+      <c r="F763">
+        <v>0</v>
+      </c>
+      <c r="G763">
+        <v>-1</v>
+      </c>
+      <c r="H763">
+        <v>1</v>
+      </c>
+      <c r="I763">
+        <v>-1</v>
+      </c>
+      <c r="J763" t="s">
+        <v>19</v>
+      </c>
+      <c r="K763">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="764" spans="1:11">
+      <c r="A764">
+        <v>1</v>
+      </c>
+      <c r="B764">
+        <v>-1</v>
+      </c>
+      <c r="C764">
+        <v>0</v>
+      </c>
+      <c r="D764">
+        <v>0</v>
+      </c>
+      <c r="E764">
+        <v>1</v>
+      </c>
+      <c r="F764">
+        <v>-1</v>
+      </c>
+      <c r="G764">
+        <v>-1</v>
+      </c>
+      <c r="H764">
+        <v>1</v>
+      </c>
+      <c r="I764">
+        <v>-1</v>
+      </c>
+      <c r="J764" t="s">
+        <v>14</v>
+      </c>
+      <c r="K764">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="765" spans="1:11">
+      <c r="A765">
+        <v>-1</v>
+      </c>
+      <c r="B765">
+        <v>0</v>
+      </c>
+      <c r="C765">
+        <v>0</v>
+      </c>
+      <c r="D765">
+        <v>0</v>
+      </c>
+      <c r="E765">
+        <v>0</v>
+      </c>
+      <c r="F765">
+        <v>0</v>
+      </c>
+      <c r="G765">
+        <v>-1</v>
+      </c>
+      <c r="H765">
+        <v>0</v>
+      </c>
+      <c r="I765">
+        <v>1</v>
+      </c>
+      <c r="J765" t="s">
+        <v>15</v>
+      </c>
+      <c r="K765">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="766" spans="1:11">
+      <c r="A766">
+        <v>0</v>
+      </c>
+      <c r="B766">
+        <v>0</v>
+      </c>
+      <c r="C766">
+        <v>1</v>
+      </c>
+      <c r="D766">
+        <v>0</v>
+      </c>
+      <c r="E766">
+        <v>0</v>
+      </c>
+      <c r="F766">
+        <v>0</v>
+      </c>
+      <c r="G766">
+        <v>-1</v>
+      </c>
+      <c r="H766">
+        <v>-1</v>
+      </c>
+      <c r="I766">
+        <v>0</v>
+      </c>
+      <c r="J766" t="s">
+        <v>11</v>
+      </c>
+      <c r="K766">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="767" spans="1:11">
+      <c r="A767">
+        <v>0</v>
+      </c>
+      <c r="B767">
+        <v>0</v>
+      </c>
+      <c r="C767">
+        <v>1</v>
+      </c>
+      <c r="D767">
+        <v>0</v>
+      </c>
+      <c r="E767">
+        <v>0</v>
+      </c>
+      <c r="F767">
+        <v>-1</v>
+      </c>
+      <c r="G767">
+        <v>-1</v>
+      </c>
+      <c r="H767">
+        <v>-1</v>
+      </c>
+      <c r="I767">
+        <v>1</v>
+      </c>
+      <c r="J767" t="s">
+        <v>15</v>
+      </c>
+      <c r="K767">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="768" spans="1:11">
+      <c r="A768">
+        <v>1</v>
+      </c>
+      <c r="B768">
+        <v>-1</v>
+      </c>
+      <c r="C768">
+        <v>-1</v>
+      </c>
+      <c r="D768">
+        <v>-1</v>
+      </c>
+      <c r="E768">
+        <v>1</v>
+      </c>
+      <c r="F768">
+        <v>0</v>
+      </c>
+      <c r="G768">
+        <v>1</v>
+      </c>
+      <c r="H768">
+        <v>1</v>
+      </c>
+      <c r="I768">
+        <v>-1</v>
+      </c>
+      <c r="J768" t="s">
+        <v>14</v>
+      </c>
+      <c r="K768">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="769" spans="1:11">
+      <c r="A769">
+        <v>1</v>
+      </c>
+      <c r="B769">
+        <v>1</v>
+      </c>
+      <c r="C769">
+        <v>-1</v>
+      </c>
+      <c r="D769">
+        <v>-1</v>
+      </c>
+      <c r="E769">
+        <v>0</v>
+      </c>
+      <c r="F769">
+        <v>-1</v>
+      </c>
+      <c r="G769">
+        <v>1</v>
+      </c>
+      <c r="H769">
+        <v>0</v>
+      </c>
+      <c r="I769">
+        <v>0</v>
+      </c>
+      <c r="J769" t="s">
+        <v>11</v>
+      </c>
+      <c r="K769">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="770" spans="1:11">
+      <c r="A770">
+        <v>0</v>
+      </c>
+      <c r="B770">
+        <v>0</v>
+      </c>
+      <c r="C770">
+        <v>0</v>
+      </c>
+      <c r="D770">
+        <v>0</v>
+      </c>
+      <c r="E770">
+        <v>0</v>
+      </c>
+      <c r="F770">
+        <v>0</v>
+      </c>
+      <c r="G770">
+        <v>-1</v>
+      </c>
+      <c r="H770">
+        <v>0</v>
+      </c>
+      <c r="I770">
+        <v>0</v>
+      </c>
+      <c r="J770" t="s">
+        <v>12</v>
+      </c>
+      <c r="K770">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="771" spans="1:11">
+      <c r="A771">
+        <v>-1</v>
+      </c>
+      <c r="B771">
+        <v>0</v>
+      </c>
+      <c r="C771">
+        <v>0</v>
+      </c>
+      <c r="D771">
+        <v>1</v>
+      </c>
+      <c r="E771">
+        <v>0</v>
+      </c>
+      <c r="F771">
+        <v>0</v>
+      </c>
+      <c r="G771">
+        <v>-1</v>
+      </c>
+      <c r="H771">
+        <v>0</v>
+      </c>
+      <c r="I771">
+        <v>0</v>
+      </c>
+      <c r="J771" t="s">
+        <v>18</v>
+      </c>
+      <c r="K771">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="772" spans="1:11">
+      <c r="A772">
+        <v>-1</v>
+      </c>
+      <c r="B772">
+        <v>-1</v>
+      </c>
+      <c r="C772">
+        <v>1</v>
+      </c>
+      <c r="D772">
+        <v>1</v>
+      </c>
+      <c r="E772">
+        <v>0</v>
+      </c>
+      <c r="F772">
+        <v>0</v>
+      </c>
+      <c r="G772">
+        <v>-1</v>
+      </c>
+      <c r="H772">
+        <v>0</v>
+      </c>
+      <c r="I772">
+        <v>0</v>
+      </c>
+      <c r="J772" t="s">
+        <v>14</v>
+      </c>
+      <c r="K772">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="773" spans="1:11">
+      <c r="A773">
+        <v>-1</v>
+      </c>
+      <c r="B773">
+        <v>-1</v>
+      </c>
+      <c r="C773">
+        <v>1</v>
+      </c>
+      <c r="D773">
+        <v>1</v>
+      </c>
+      <c r="E773">
+        <v>0</v>
+      </c>
+      <c r="F773">
+        <v>1</v>
+      </c>
+      <c r="G773">
+        <v>-1</v>
+      </c>
+      <c r="H773">
+        <v>0</v>
+      </c>
+      <c r="I773">
+        <v>-1</v>
+      </c>
+      <c r="J773" t="s">
+        <v>13</v>
+      </c>
+      <c r="K773">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="774" spans="1:11">
+      <c r="A774">
+        <v>1</v>
+      </c>
+      <c r="B774">
+        <v>1</v>
+      </c>
+      <c r="C774">
+        <v>-1</v>
+      </c>
+      <c r="D774">
+        <v>-1</v>
+      </c>
+      <c r="E774">
+        <v>0</v>
+      </c>
+      <c r="F774">
+        <v>0</v>
+      </c>
+      <c r="G774">
+        <v>1</v>
+      </c>
+      <c r="H774">
+        <v>0</v>
+      </c>
+      <c r="I774">
+        <v>-1</v>
+      </c>
+      <c r="J774" t="s">
+        <v>17</v>
+      </c>
+      <c r="K774">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="775" spans="1:11">
+      <c r="A775">
+        <v>1</v>
+      </c>
+      <c r="B775">
+        <v>1</v>
+      </c>
+      <c r="C775">
+        <v>-1</v>
+      </c>
+      <c r="D775">
+        <v>-1</v>
+      </c>
+      <c r="E775">
+        <v>-1</v>
+      </c>
+      <c r="F775">
+        <v>0</v>
+      </c>
+      <c r="G775">
+        <v>1</v>
+      </c>
+      <c r="H775">
+        <v>1</v>
+      </c>
+      <c r="I775">
+        <v>-1</v>
+      </c>
+      <c r="J775" t="s">
+        <v>14</v>
+      </c>
+      <c r="K775">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="776" spans="1:11">
+      <c r="A776">
+        <v>1</v>
+      </c>
+      <c r="B776">
+        <v>0</v>
+      </c>
+      <c r="C776">
+        <v>-1</v>
+      </c>
+      <c r="D776">
+        <v>-1</v>
+      </c>
+      <c r="E776">
+        <v>-1</v>
+      </c>
+      <c r="F776">
+        <v>1</v>
+      </c>
+      <c r="G776">
+        <v>1</v>
+      </c>
+      <c r="H776">
+        <v>1</v>
+      </c>
+      <c r="I776">
+        <v>-1</v>
+      </c>
+      <c r="J776" t="s">
+        <v>19</v>
+      </c>
+      <c r="K776">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="777" spans="1:11">
+      <c r="A777">
+        <v>1</v>
+      </c>
+      <c r="B777">
+        <v>0</v>
+      </c>
+      <c r="C777">
+        <v>-1</v>
+      </c>
+      <c r="D777">
+        <v>-1</v>
+      </c>
+      <c r="E777">
+        <v>0</v>
+      </c>
+      <c r="F777">
+        <v>1</v>
+      </c>
+      <c r="G777">
+        <v>1</v>
+      </c>
+      <c r="H777">
+        <v>0</v>
+      </c>
+      <c r="I777">
+        <v>-1</v>
+      </c>
+      <c r="J777" t="s">
+        <v>19</v>
+      </c>
+      <c r="K777">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="778" spans="1:11">
+      <c r="A778">
+        <v>1</v>
+      </c>
+      <c r="B778">
+        <v>1</v>
+      </c>
+      <c r="C778">
+        <v>-1</v>
+      </c>
+      <c r="D778">
+        <v>-1</v>
+      </c>
+      <c r="E778">
+        <v>0</v>
+      </c>
+      <c r="F778">
+        <v>1</v>
+      </c>
+      <c r="G778">
+        <v>1</v>
+      </c>
+      <c r="H778">
+        <v>-1</v>
+      </c>
+      <c r="I778">
+        <v>-1</v>
+      </c>
+      <c r="J778" t="s">
+        <v>13</v>
+      </c>
+      <c r="K778">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="779" spans="1:11">
+      <c r="A779">
+        <v>1</v>
+      </c>
+      <c r="B779">
+        <v>1</v>
+      </c>
+      <c r="C779">
+        <v>-1</v>
+      </c>
+      <c r="D779">
+        <v>-1</v>
+      </c>
+      <c r="E779">
+        <v>-1</v>
+      </c>
+      <c r="F779">
+        <v>1</v>
+      </c>
+      <c r="G779">
+        <v>1</v>
+      </c>
+      <c r="H779">
+        <v>0</v>
+      </c>
+      <c r="I779">
+        <v>-1</v>
+      </c>
+      <c r="J779" t="s">
+        <v>17</v>
+      </c>
+      <c r="K779">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="780" spans="1:11">
+      <c r="A780">
+        <v>-1</v>
+      </c>
+      <c r="B780">
+        <v>0</v>
+      </c>
+      <c r="C780">
+        <v>0</v>
+      </c>
+      <c r="D780">
+        <v>1</v>
+      </c>
+      <c r="E780">
+        <v>0</v>
+      </c>
+      <c r="F780">
+        <v>0</v>
+      </c>
+      <c r="G780">
+        <v>-1</v>
+      </c>
+      <c r="H780">
+        <v>0</v>
+      </c>
+      <c r="I780">
+        <v>0</v>
+      </c>
+      <c r="J780" t="s">
+        <v>13</v>
+      </c>
+      <c r="K780">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="781" spans="1:11">
+      <c r="A781">
+        <v>-1</v>
+      </c>
+      <c r="B781">
+        <v>0</v>
+      </c>
+      <c r="C781">
+        <v>-1</v>
+      </c>
+      <c r="D781">
+        <v>1</v>
+      </c>
+      <c r="E781">
+        <v>1</v>
+      </c>
+      <c r="F781">
+        <v>0</v>
+      </c>
+      <c r="G781">
+        <v>-1</v>
+      </c>
+      <c r="H781">
+        <v>0</v>
+      </c>
+      <c r="I781">
+        <v>0</v>
+      </c>
+      <c r="J781" t="s">
+        <v>14</v>
+      </c>
+      <c r="K781">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="782" spans="1:11">
+      <c r="A782">
+        <v>1</v>
+      </c>
+      <c r="B782">
+        <v>1</v>
+      </c>
+      <c r="C782">
+        <v>-1</v>
+      </c>
+      <c r="D782">
+        <v>-1</v>
+      </c>
+      <c r="E782">
+        <v>-1</v>
+      </c>
+      <c r="F782">
+        <v>0</v>
+      </c>
+      <c r="G782">
+        <v>1</v>
+      </c>
+      <c r="H782">
+        <v>-1</v>
+      </c>
+      <c r="I782">
+        <v>1</v>
+      </c>
+      <c r="J782" t="s">
+        <v>14</v>
+      </c>
+      <c r="K782">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="783" spans="1:11">
+      <c r="A783">
+        <v>-1</v>
+      </c>
+      <c r="B783">
+        <v>0</v>
+      </c>
+      <c r="C783">
+        <v>-1</v>
+      </c>
+      <c r="D783">
+        <v>1</v>
+      </c>
+      <c r="E783">
+        <v>1</v>
+      </c>
+      <c r="F783">
+        <v>-1</v>
+      </c>
+      <c r="G783">
+        <v>1</v>
+      </c>
+      <c r="H783">
+        <v>-1</v>
+      </c>
+      <c r="I783">
+        <v>1</v>
+      </c>
+      <c r="J783" t="s">
+        <v>19</v>
+      </c>
+      <c r="K783">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="784" spans="1:11">
+      <c r="A784">
+        <v>0</v>
+      </c>
+      <c r="B784">
+        <v>1</v>
+      </c>
+      <c r="C784">
+        <v>-1</v>
+      </c>
+      <c r="D784">
+        <v>-1</v>
+      </c>
+      <c r="E784">
+        <v>-1</v>
+      </c>
+      <c r="F784">
+        <v>1</v>
+      </c>
+      <c r="G784">
+        <v>1</v>
+      </c>
+      <c r="H784">
+        <v>1</v>
+      </c>
+      <c r="I784">
+        <v>-1</v>
+      </c>
+      <c r="J784" t="s">
+        <v>15</v>
+      </c>
+      <c r="K784">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="785" spans="1:11">
+      <c r="A785">
+        <v>-1</v>
+      </c>
+      <c r="B785">
+        <v>1</v>
+      </c>
+      <c r="C785">
+        <v>-1</v>
+      </c>
+      <c r="D785">
+        <v>-1</v>
+      </c>
+      <c r="E785">
+        <v>1</v>
+      </c>
+      <c r="F785">
+        <v>1</v>
+      </c>
+      <c r="G785">
+        <v>1</v>
+      </c>
+      <c r="H785">
+        <v>-1</v>
+      </c>
+      <c r="I785">
+        <v>0</v>
+      </c>
+      <c r="J785" t="s">
+        <v>11</v>
+      </c>
+      <c r="K785">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="786" spans="1:11">
+      <c r="A786">
+        <v>-1</v>
+      </c>
+      <c r="B786">
+        <v>1</v>
+      </c>
+      <c r="C786">
+        <v>-1</v>
+      </c>
+      <c r="D786">
+        <v>0</v>
+      </c>
+      <c r="E786">
+        <v>-1</v>
+      </c>
+      <c r="F786">
+        <v>1</v>
+      </c>
+      <c r="G786">
+        <v>1</v>
+      </c>
+      <c r="H786">
+        <v>-1</v>
+      </c>
+      <c r="I786">
+        <v>1</v>
+      </c>
+      <c r="J786" t="s">
+        <v>12</v>
+      </c>
+      <c r="K786">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="787" spans="1:11">
+      <c r="A787">
+        <v>1</v>
+      </c>
+      <c r="B787">
+        <v>-1</v>
+      </c>
+      <c r="C787">
+        <v>-1</v>
+      </c>
+      <c r="D787">
+        <v>-1</v>
+      </c>
+      <c r="E787">
+        <v>0</v>
+      </c>
+      <c r="F787">
+        <v>1</v>
+      </c>
+      <c r="G787">
+        <v>1</v>
+      </c>
+      <c r="H787">
+        <v>1</v>
+      </c>
+      <c r="I787">
+        <v>-1</v>
+      </c>
+      <c r="J787" t="s">
+        <v>13</v>
+      </c>
+      <c r="K787">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="788" spans="1:11">
+      <c r="A788">
+        <v>-1</v>
+      </c>
+      <c r="B788">
+        <v>0</v>
+      </c>
+      <c r="C788">
+        <v>0</v>
+      </c>
+      <c r="D788">
+        <v>1</v>
+      </c>
+      <c r="E788">
+        <v>0</v>
+      </c>
+      <c r="F788">
+        <v>0</v>
+      </c>
+      <c r="G788">
+        <v>-1</v>
+      </c>
+      <c r="H788">
+        <v>0</v>
+      </c>
+      <c r="I788">
+        <v>0</v>
+      </c>
+      <c r="J788" t="s">
+        <v>17</v>
+      </c>
+      <c r="K788">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="789" spans="1:11">
+      <c r="A789">
+        <v>-1</v>
+      </c>
+      <c r="B789">
+        <v>0</v>
+      </c>
+      <c r="C789">
+        <v>0</v>
+      </c>
+      <c r="D789">
+        <v>1</v>
+      </c>
+      <c r="E789">
+        <v>0</v>
+      </c>
+      <c r="F789">
+        <v>0</v>
+      </c>
+      <c r="G789">
+        <v>-1</v>
+      </c>
+      <c r="H789">
+        <v>1</v>
+      </c>
+      <c r="I789">
+        <v>-1</v>
+      </c>
+      <c r="J789" t="s">
+        <v>13</v>
+      </c>
+      <c r="K789">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="790" spans="1:11">
+      <c r="A790">
+        <v>-1</v>
+      </c>
+      <c r="B790">
+        <v>1</v>
+      </c>
+      <c r="C790">
+        <v>-1</v>
+      </c>
+      <c r="D790">
+        <v>1</v>
+      </c>
+      <c r="E790">
+        <v>1</v>
+      </c>
+      <c r="F790">
+        <v>-1</v>
+      </c>
+      <c r="G790">
+        <v>1</v>
+      </c>
+      <c r="H790">
+        <v>-1</v>
+      </c>
+      <c r="I790">
+        <v>0</v>
+      </c>
+      <c r="J790" t="s">
+        <v>11</v>
+      </c>
+      <c r="K790">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="791" spans="1:11">
+      <c r="A791">
+        <v>-1</v>
+      </c>
+      <c r="B791">
+        <v>0</v>
+      </c>
+      <c r="C791">
+        <v>0</v>
+      </c>
+      <c r="D791">
+        <v>1</v>
+      </c>
+      <c r="E791">
+        <v>0</v>
+      </c>
+      <c r="F791">
+        <v>0</v>
+      </c>
+      <c r="G791">
+        <v>-1</v>
+      </c>
+      <c r="H791">
+        <v>0</v>
+      </c>
+      <c r="I791">
+        <v>0</v>
+      </c>
+      <c r="J791" t="s">
+        <v>11</v>
+      </c>
+      <c r="K791">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="792" spans="1:11">
+      <c r="A792">
+        <v>-1</v>
+      </c>
+      <c r="B792">
+        <v>-1</v>
+      </c>
+      <c r="C792">
+        <v>0</v>
+      </c>
+      <c r="D792">
+        <v>1</v>
+      </c>
+      <c r="E792">
+        <v>0</v>
+      </c>
+      <c r="F792">
+        <v>0</v>
+      </c>
+      <c r="G792">
+        <v>-1</v>
+      </c>
+      <c r="H792">
+        <v>0</v>
+      </c>
+      <c r="I792">
+        <v>1</v>
+      </c>
+      <c r="J792" t="s">
+        <v>18</v>
+      </c>
+      <c r="K792">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="793" spans="1:11">
+      <c r="A793">
+        <v>-1</v>
+      </c>
+      <c r="B793">
+        <v>-1</v>
+      </c>
+      <c r="C793">
+        <v>1</v>
+      </c>
+      <c r="D793">
+        <v>1</v>
+      </c>
+      <c r="E793">
+        <v>0</v>
+      </c>
+      <c r="F793">
+        <v>0</v>
+      </c>
+      <c r="G793">
+        <v>-1</v>
+      </c>
+      <c r="H793">
+        <v>-1</v>
+      </c>
+      <c r="I793">
+        <v>1</v>
+      </c>
+      <c r="J793" t="s">
+        <v>14</v>
+      </c>
+      <c r="K793">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="794" spans="1:11">
+      <c r="A794">
+        <v>0</v>
+      </c>
+      <c r="B794">
+        <v>0</v>
+      </c>
+      <c r="C794">
+        <v>0</v>
+      </c>
+      <c r="D794">
+        <v>0</v>
+      </c>
+      <c r="E794">
+        <v>0</v>
+      </c>
+      <c r="F794">
+        <v>0</v>
+      </c>
+      <c r="G794">
+        <v>-1</v>
+      </c>
+      <c r="H794">
+        <v>0</v>
+      </c>
+      <c r="I794">
+        <v>0</v>
+      </c>
+      <c r="J794" t="s">
+        <v>11</v>
+      </c>
+      <c r="K794">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="795" spans="1:11">
+      <c r="A795">
+        <v>-1</v>
+      </c>
+      <c r="B795">
+        <v>0</v>
+      </c>
+      <c r="C795">
+        <v>0</v>
+      </c>
+      <c r="D795">
+        <v>0</v>
+      </c>
+      <c r="E795">
+        <v>0</v>
+      </c>
+      <c r="F795">
+        <v>0</v>
+      </c>
+      <c r="G795">
+        <v>-1</v>
+      </c>
+      <c r="H795">
+        <v>0</v>
+      </c>
+      <c r="I795">
+        <v>1</v>
+      </c>
+      <c r="J795" t="s">
+        <v>12</v>
+      </c>
+      <c r="K795">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="796" spans="1:11">
+      <c r="A796">
+        <v>1</v>
+      </c>
+      <c r="B796">
+        <v>1</v>
+      </c>
+      <c r="C796">
+        <v>-1</v>
+      </c>
+      <c r="D796">
+        <v>-1</v>
+      </c>
+      <c r="E796">
+        <v>-1</v>
+      </c>
+      <c r="F796">
+        <v>0</v>
+      </c>
+      <c r="G796">
+        <v>1</v>
+      </c>
+      <c r="H796">
+        <v>0</v>
+      </c>
+      <c r="I796">
+        <v>0</v>
+      </c>
+      <c r="J796" t="s">
+        <v>17</v>
+      </c>
+      <c r="K796">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="797" spans="1:11">
+      <c r="A797">
+        <v>0</v>
+      </c>
+      <c r="B797">
+        <v>1</v>
+      </c>
+      <c r="C797">
+        <v>-1</v>
+      </c>
+      <c r="D797">
+        <v>-1</v>
+      </c>
+      <c r="E797">
+        <v>-1</v>
+      </c>
+      <c r="F797">
+        <v>1</v>
+      </c>
+      <c r="G797">
+        <v>1</v>
+      </c>
+      <c r="H797">
+        <v>-1</v>
+      </c>
+      <c r="I797">
+        <v>1</v>
+      </c>
+      <c r="J797" t="s">
+        <v>15</v>
+      </c>
+      <c r="K797">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="798" spans="1:11">
+      <c r="A798">
+        <v>0</v>
+      </c>
+      <c r="B798">
+        <v>0</v>
+      </c>
+      <c r="C798">
+        <v>0</v>
+      </c>
+      <c r="D798">
+        <v>0</v>
+      </c>
+      <c r="E798">
+        <v>0</v>
+      </c>
+      <c r="F798">
+        <v>0</v>
+      </c>
+      <c r="G798">
+        <v>-1</v>
+      </c>
+      <c r="H798">
+        <v>0</v>
+      </c>
+      <c r="I798">
+        <v>0</v>
+      </c>
+      <c r="J798" t="s">
+        <v>17</v>
+      </c>
+      <c r="K798">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="799" spans="1:11">
+      <c r="A799">
+        <v>0</v>
+      </c>
+      <c r="B799">
+        <v>0</v>
+      </c>
+      <c r="C799">
+        <v>-1</v>
+      </c>
+      <c r="D799">
+        <v>0</v>
+      </c>
+      <c r="E799">
+        <v>0</v>
+      </c>
+      <c r="F799">
+        <v>0</v>
+      </c>
+      <c r="G799">
+        <v>-1</v>
+      </c>
+      <c r="H799">
+        <v>1</v>
+      </c>
+      <c r="I799">
+        <v>0</v>
+      </c>
+      <c r="J799" t="s">
+        <v>13</v>
+      </c>
+      <c r="K799">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="800" spans="1:11">
+      <c r="A800">
+        <v>0</v>
+      </c>
+      <c r="B800">
+        <v>-1</v>
+      </c>
+      <c r="C800">
+        <v>-1</v>
+      </c>
+      <c r="D800">
+        <v>0</v>
+      </c>
+      <c r="E800">
+        <v>1</v>
+      </c>
+      <c r="F800">
+        <v>0</v>
+      </c>
+      <c r="G800">
+        <v>-1</v>
+      </c>
+      <c r="H800">
+        <v>1</v>
+      </c>
+      <c r="I800">
+        <v>0</v>
+      </c>
+      <c r="J800" t="s">
+        <v>15</v>
+      </c>
+      <c r="K800">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="801" spans="1:11">
+      <c r="A801">
+        <v>1</v>
+      </c>
+      <c r="B801">
+        <v>-1</v>
+      </c>
+      <c r="C801">
+        <v>-1</v>
+      </c>
+      <c r="D801">
+        <v>0</v>
+      </c>
+      <c r="E801">
+        <v>1</v>
+      </c>
+      <c r="F801">
+        <v>-1</v>
+      </c>
+      <c r="G801">
+        <v>-1</v>
+      </c>
+      <c r="H801">
+        <v>1</v>
+      </c>
+      <c r="I801">
+        <v>0</v>
+      </c>
+      <c r="J801" t="s">
+        <v>11</v>
+      </c>
+      <c r="K801">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="802" spans="1:11">
+      <c r="A802">
+        <v>1</v>
+      </c>
+      <c r="B802">
+        <v>0</v>
+      </c>
+      <c r="C802">
+        <v>-1</v>
+      </c>
+      <c r="D802">
+        <v>-1</v>
+      </c>
+      <c r="E802">
+        <v>-1</v>
+      </c>
+      <c r="F802">
+        <v>1</v>
+      </c>
+      <c r="G802">
+        <v>1</v>
+      </c>
+      <c r="H802">
+        <v>-1</v>
+      </c>
+      <c r="I802">
+        <v>1</v>
+      </c>
+      <c r="J802" t="s">
+        <v>19</v>
+      </c>
+      <c r="K802">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="803" spans="1:11">
+      <c r="A803">
+        <v>1</v>
+      </c>
+      <c r="B803">
+        <v>-1</v>
+      </c>
+      <c r="C803">
+        <v>1</v>
+      </c>
+      <c r="D803">
+        <v>-1</v>
+      </c>
+      <c r="E803">
+        <v>-1</v>
+      </c>
+      <c r="F803">
+        <v>0</v>
+      </c>
+      <c r="G803">
+        <v>1</v>
+      </c>
+      <c r="H803">
+        <v>0</v>
+      </c>
+      <c r="I803">
+        <v>0</v>
+      </c>
+      <c r="J803" t="s">
+        <v>17</v>
+      </c>
+      <c r="K803">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="804" spans="1:11">
+      <c r="A804">
+        <v>1</v>
+      </c>
+      <c r="B804">
+        <v>-1</v>
+      </c>
+      <c r="C804">
+        <v>1</v>
+      </c>
+      <c r="D804">
+        <v>-1</v>
+      </c>
+      <c r="E804">
+        <v>-1</v>
+      </c>
+      <c r="F804">
+        <v>0</v>
+      </c>
+      <c r="G804">
+        <v>1</v>
+      </c>
+      <c r="H804">
+        <v>1</v>
+      </c>
+      <c r="I804">
+        <v>-1</v>
+      </c>
+      <c r="J804" t="s">
+        <v>14</v>
+      </c>
+      <c r="K804">
         <v>1</v>
       </c>
     </row>

</xml_diff>